<commit_message>
Added 0208 for TICC-126
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v7.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v7.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$L$84</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="439">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1493,6 +1493,36 @@
   </si>
   <si>
     <t>Replaced by 0204</t>
+  </si>
+  <si>
+    <t>0208</t>
+  </si>
+  <si>
+    <t>Numero d'entreprise / ondernemingsnummer / Unternehmensnummer</t>
+  </si>
+  <si>
+    <t>Banque-Carrefour des Entreprises (BCE) / Kruispuntbank van Ondernemingen (KBO) / Zentrale Datenbank der Unternehmen (ZOU)
+Service public fédéral Economie, P.M.E. Classes moyennes et Energie</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>BE:BCE</t>
+  </si>
+  <si>
+    <t>10 numeric characters.
+1. Enterprise identification number: the first digit has to be "0" or "1"
+2. Establishment unit identification number: the first digit has to be "2".
+The two last characters are check digits. They are the result of the following computation: 97 - ((8 first digits) modulo 97).</t>
+  </si>
+  <si>
+    <t>The identification number can be displayed in the following ways:
+For enterprise numbers:
+- a group of four digits, then two groups of three digits, each group separated by a dot. Example: 1234.456.789
+- one digit, then three groups of three digits, each separated by a dot. Example: 1.234.456.789
+For establishment unit numbers:
+- one digit, then three groups of three digits, each separated by a dot. Example: 2.123.456.789</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1586,8 +1616,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1598,7 +1626,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1894,28 +1931,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AML83"/>
+  <dimension ref="A1:AML84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="67.81640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="34.1796875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="30.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="14.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="62.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="14.140625" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1">
@@ -1937,7 +1975,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1956,7 +1994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="87">
+    <row r="2" spans="1:12" ht="90">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1975,14 +2013,14 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>390</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1992,7 +2030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="43.5">
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2011,21 +2049,21 @@
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -2044,21 +2082,21 @@
       <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="G4" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="130.5">
+    <row r="5" spans="1:12" ht="150">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2077,14 +2115,14 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="G5" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2094,7 +2132,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="87">
+    <row r="6" spans="1:12" ht="105">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -2113,14 +2151,14 @@
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="G6" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -2130,7 +2168,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="29">
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -2149,14 +2187,14 @@
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -2166,7 +2204,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="145">
+    <row r="8" spans="1:12" ht="195">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -2185,18 +2223,18 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="174">
+    <row r="9" spans="1:12" ht="180">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -2215,21 +2253,21 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="159.5">
+    <row r="10" spans="1:12" ht="210">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -2248,21 +2286,21 @@
       <c r="F10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="G10" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.5">
+    <row r="11" spans="1:12" ht="45">
       <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
@@ -2281,21 +2319,21 @@
       <c r="F11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="G11" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29">
+    <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -2314,14 +2352,14 @@
       <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -2347,21 +2385,21 @@
       <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="10" t="s">
+      <c r="G13" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="159.5">
+    <row r="14" spans="1:12" ht="210">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2380,14 +2418,14 @@
       <c r="F14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="10" t="s">
+      <c r="G14" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="8" t="s">
         <v>84</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -2397,7 +2435,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="145">
+    <row r="15" spans="1:12" ht="150">
       <c r="A15" s="1" t="s">
         <v>345</v>
       </c>
@@ -2416,14 +2454,14 @@
       <c r="F15" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="G15" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="8" t="s">
         <v>343</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -2449,18 +2487,18 @@
       <c r="F16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="10" t="s">
+      <c r="G16" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:12 1026:1026" ht="116">
+    <row r="17" spans="1:12 1026:1026" ht="150">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -2479,14 +2517,14 @@
       <c r="F17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="10" t="s">
+      <c r="G17" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>392</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -2496,7 +2534,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="18" spans="1:12 1026:1026" ht="101.5">
+    <row r="18" spans="1:12 1026:1026" ht="105">
       <c r="A18" s="1" t="s">
         <v>94</v>
       </c>
@@ -2515,14 +2553,14 @@
       <c r="F18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="10" t="s">
+      <c r="G18" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -2532,7 +2570,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="19" spans="1:12 1026:1026" ht="58">
+    <row r="19" spans="1:12 1026:1026" ht="60">
       <c r="A19" s="1" t="s">
         <v>99</v>
       </c>
@@ -2551,21 +2589,21 @@
       <c r="F19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="10" t="s">
+      <c r="G19" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="1:12 1026:1026" ht="43.5">
+    <row r="20" spans="1:12 1026:1026" ht="45">
       <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
@@ -2584,18 +2622,18 @@
       <c r="F20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="10" t="s">
+      <c r="G20" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:12 1026:1026" ht="87">
+    <row r="21" spans="1:12 1026:1026" ht="105">
       <c r="A21" s="1" t="s">
         <v>112</v>
       </c>
@@ -2614,21 +2652,21 @@
       <c r="F21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="10" t="s">
+      <c r="G21" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="8" t="s">
         <v>393</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="22" spans="1:12 1026:1026" ht="87">
+    <row r="22" spans="1:12 1026:1026" ht="105">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2647,18 +2685,18 @@
       <c r="F22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="10" t="s">
+      <c r="G22" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="8" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="1:12 1026:1026" ht="29">
+    <row r="23" spans="1:12 1026:1026" ht="30">
       <c r="A23" s="1" t="s">
         <v>351</v>
       </c>
@@ -2677,14 +2715,14 @@
       <c r="F23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10" t="s">
+      <c r="G23" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="8" t="s">
         <v>354</v>
       </c>
     </row>
@@ -2707,18 +2745,18 @@
       <c r="F24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="10" t="s">
+      <c r="G24" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="8" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="25" spans="1:12 1026:1026" ht="72.5">
+    <row r="25" spans="1:12 1026:1026" ht="90">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -2737,21 +2775,21 @@
       <c r="F25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="10" t="s">
+      <c r="G25" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="26" spans="1:12 1026:1026">
+    <row r="26" spans="1:12 1026:1026" ht="30">
       <c r="A26" s="1" t="s">
         <v>360</v>
       </c>
@@ -2770,23 +2808,23 @@
       <c r="F26" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G26" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="G26" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K26" s="7"/>
+      <c r="K26" s="5"/>
       <c r="L26" s="1" t="s">
         <v>366</v>
       </c>
       <c r="AML26" s="1"/>
     </row>
-    <row r="27" spans="1:12 1026:1026" ht="43.5">
+    <row r="27" spans="1:12 1026:1026" ht="45">
       <c r="A27" s="1" t="s">
         <v>367</v>
       </c>
@@ -2805,1383 +2843,1415 @@
       <c r="F27" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G27" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="10" t="s">
+      <c r="G27" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="K27" s="7"/>
+      <c r="K27" s="5"/>
       <c r="L27" s="1" t="s">
         <v>373</v>
       </c>
       <c r="AML27" s="1"/>
     </row>
-    <row r="28" spans="1:12 1026:1026" ht="29">
+    <row r="28" spans="1:12 1026:1026" ht="165">
       <c r="A28" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G28" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="AML28" s="1"/>
+    </row>
+    <row r="29" spans="1:12 1026:1026" ht="30">
+      <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12 1026:1026" ht="29">
-      <c r="A29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12 1026:1026" ht="29">
+      <c r="G29" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12 1026:1026" ht="30">
       <c r="A30" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="9" t="b">
+      <c r="G30" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12 1026:1026" ht="43.5">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12 1026:1026" ht="30">
       <c r="A31" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="9" t="b">
+      <c r="G31" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12 1026:1026">
+    </row>
+    <row r="32" spans="1:12 1026:1026" ht="45">
       <c r="A32" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="9" t="b">
+      <c r="G32" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="101.5">
+        <v>138</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="9" t="b">
+      <c r="G33" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="58">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="105">
       <c r="A34" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>104</v>
+      <c r="G34" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>407</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="29">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="60">
       <c r="A35" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>348</v>
+        <v>151</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="9" t="b">
+      <c r="G35" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30">
+      <c r="A36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:12">
+      <c r="A37" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="72.5">
-      <c r="A37" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37"/>
       <c r="F37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="9" t="b">
+      <c r="G37" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="90">
+      <c r="A38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I38" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:12" ht="30">
+      <c r="A39" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="29">
-      <c r="A39" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="29">
+      <c r="G39" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30">
       <c r="A40" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40"/>
+        <v>170</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="9" t="b">
+      <c r="G40" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="29">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30">
       <c r="A41" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="9" t="b">
+      <c r="G41" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30">
+      <c r="A42" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="87">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:12" ht="105">
+      <c r="A43" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="9" t="b">
+      <c r="G43" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I42" s="10" t="s">
+      <c r="I43" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J43" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="72.5">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:12" ht="75">
+      <c r="A44" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G43" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="10" t="s">
+      <c r="G44" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="8" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:12">
+      <c r="A45" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E44"/>
-      <c r="F44" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G44" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="29">
-      <c r="A45" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G45" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="29">
+      <c r="G45" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="30">
       <c r="A46" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G46" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30">
+      <c r="A47" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G46" s="9" t="b">
+      <c r="G47" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:12">
+      <c r="A48" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E47"/>
-      <c r="F47" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G47" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E48"/>
+      <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G48" s="9" t="b">
+      <c r="G48" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="5" t="s">
-        <v>205</v>
+      <c r="A49" s="10" t="s">
+        <v>201</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E49"/>
+        <v>204</v>
+      </c>
+      <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G49" s="9" t="b">
+      <c r="G49" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="5" t="s">
-        <v>209</v>
+      <c r="A50" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>107</v>
+        <v>207</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E50"/>
+        <v>208</v>
+      </c>
+      <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G50" s="9" t="b">
+      <c r="G50" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="5" t="s">
-        <v>212</v>
+      <c r="A51" s="10" t="s">
+        <v>209</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>214</v>
+        <v>107</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E51"/>
+        <v>211</v>
+      </c>
+      <c r="E51" s="9"/>
       <c r="F51" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G51" s="9" t="b">
+      <c r="G51" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="5" t="s">
-        <v>216</v>
+      <c r="A52" s="10" t="s">
+        <v>212</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E52"/>
+        <v>215</v>
+      </c>
+      <c r="E52" s="9"/>
       <c r="F52" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G52" s="9" t="b">
+      <c r="G52" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="5" t="s">
-        <v>220</v>
+      <c r="A53" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G53" s="9" t="b">
+      <c r="G53" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="5" t="s">
-        <v>224</v>
+      <c r="A54" s="10" t="s">
+        <v>220</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E54"/>
+        <v>223</v>
+      </c>
       <c r="F54" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G54" s="9" t="b">
+      <c r="G54" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="5" t="s">
-        <v>228</v>
+      <c r="A55" s="10" t="s">
+        <v>224</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E55"/>
+        <v>227</v>
+      </c>
+      <c r="E55" s="9"/>
       <c r="F55" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G55" s="9" t="b">
+      <c r="G55" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="5" t="s">
-        <v>232</v>
+      <c r="A56" s="10" t="s">
+        <v>228</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>96</v>
+        <v>230</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E56"/>
+        <v>231</v>
+      </c>
+      <c r="E56" s="9"/>
       <c r="F56" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G56" s="9" t="b">
+      <c r="G56" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="6" t="s">
-        <v>235</v>
+      <c r="A57" s="10" t="s">
+        <v>232</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>237</v>
+        <v>96</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E57"/>
+        <v>234</v>
+      </c>
+      <c r="E57" s="9"/>
       <c r="F57" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G57" s="9" t="b">
+      <c r="G57" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="6" t="s">
-        <v>239</v>
+      <c r="A58" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E58"/>
+        <v>238</v>
+      </c>
+      <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G58" s="9" t="b">
+      <c r="G58" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="6" t="s">
-        <v>243</v>
+      <c r="A59" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E59"/>
+        <v>242</v>
+      </c>
+      <c r="E59" s="9"/>
       <c r="F59" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G59" s="9" t="b">
+      <c r="G59" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="6" t="s">
-        <v>247</v>
+      <c r="A60" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E60"/>
+        <v>246</v>
+      </c>
+      <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G60" s="9" t="b">
+      <c r="G60" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="6" t="s">
-        <v>251</v>
+      <c r="A61" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E61"/>
+        <v>250</v>
+      </c>
+      <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G61" s="9" t="b">
+      <c r="G61" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="6" t="s">
-        <v>255</v>
+      <c r="A62" s="11" t="s">
+        <v>251</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>124</v>
+        <v>253</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E62"/>
+        <v>254</v>
+      </c>
+      <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G62" s="9" t="b">
+      <c r="G62" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="6" t="s">
-        <v>258</v>
+      <c r="A63" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>260</v>
+        <v>124</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E63"/>
+        <v>257</v>
+      </c>
+      <c r="E63" s="9"/>
       <c r="F63" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G63" s="9" t="b">
+      <c r="G63" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="6" t="s">
-        <v>262</v>
+      <c r="A64" s="11" t="s">
+        <v>258</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E64"/>
+        <v>261</v>
+      </c>
+      <c r="E64" s="9"/>
       <c r="F64" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G64" s="9" t="b">
+      <c r="G64" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="6" t="s">
-        <v>266</v>
+      <c r="A65" s="11" t="s">
+        <v>262</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E65"/>
+        <v>265</v>
+      </c>
+      <c r="E65" s="9"/>
       <c r="F65" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G65" s="9" t="b">
+      <c r="G65" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="6" t="s">
-        <v>270</v>
+      <c r="A66" s="11" t="s">
+        <v>266</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E66"/>
+        <v>269</v>
+      </c>
+      <c r="E66" s="9"/>
       <c r="F66" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G66" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="29">
-      <c r="A67" s="6" t="s">
-        <v>274</v>
+      <c r="G66" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="11" t="s">
+        <v>270</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E67"/>
+        <v>273</v>
+      </c>
+      <c r="E67" s="9"/>
       <c r="F67" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G67" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="6" t="s">
-        <v>278</v>
+      <c r="G67" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="30">
+      <c r="A68" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E68"/>
+        <v>277</v>
+      </c>
+      <c r="E68" s="9"/>
       <c r="F68" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G68" s="9" t="b">
+      <c r="G68" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="6" t="s">
-        <v>282</v>
+      <c r="A69" s="11" t="s">
+        <v>278</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>59</v>
+        <v>280</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E69"/>
+        <v>281</v>
+      </c>
+      <c r="E69" s="9"/>
       <c r="F69" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G69" s="9" t="b">
+      <c r="G69" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="6" t="s">
-        <v>285</v>
+      <c r="A70" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>287</v>
+        <v>59</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E70"/>
+        <v>284</v>
+      </c>
+      <c r="E70" s="9"/>
       <c r="F70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G70" s="9" t="b">
+      <c r="G70" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="6" t="s">
-        <v>289</v>
+      <c r="A71" s="11" t="s">
+        <v>285</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E71"/>
+        <v>288</v>
+      </c>
+      <c r="E71" s="9"/>
       <c r="F71" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G71" s="9" t="b">
+      <c r="G71" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="6" t="s">
-        <v>293</v>
+      <c r="A72" s="11" t="s">
+        <v>289</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E72"/>
+        <v>292</v>
+      </c>
+      <c r="E72" s="9"/>
       <c r="F72" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G72" s="9" t="b">
+      <c r="G72" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="6" t="s">
-        <v>297</v>
+      <c r="A73" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E73"/>
+        <v>296</v>
+      </c>
+      <c r="E73" s="9"/>
       <c r="F73" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G73" s="9" t="b">
+      <c r="G73" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:12">
-      <c r="A74" s="6" t="s">
-        <v>301</v>
+      <c r="A74" s="11" t="s">
+        <v>297</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E74"/>
+        <v>300</v>
+      </c>
+      <c r="E74" s="9"/>
       <c r="F74" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G74" s="9" t="b">
+      <c r="G74" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="6" t="s">
-        <v>305</v>
+      <c r="A75" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E75"/>
+        <v>304</v>
+      </c>
+      <c r="E75" s="9"/>
       <c r="F75" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G75" s="9" t="b">
+      <c r="G75" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="6" t="s">
-        <v>309</v>
+      <c r="A76" s="11" t="s">
+        <v>305</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>312</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="E76" s="9"/>
       <c r="F76" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G76" s="9" t="b">
+      <c r="G76" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="6" t="s">
-        <v>313</v>
+      <c r="A77" s="11" t="s">
+        <v>309</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E77"/>
+        <v>312</v>
+      </c>
       <c r="F77" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G77" s="9" t="b">
+      <c r="G77" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="6" t="s">
-        <v>317</v>
+      <c r="A78" s="11" t="s">
+        <v>313</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E78"/>
+        <v>316</v>
+      </c>
+      <c r="E78" s="9"/>
       <c r="F78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G78" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="1" t="s">
+      <c r="G78" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="30">
+      <c r="A79" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="F79" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G79" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="G79" s="9" t="b">
+      <c r="G80" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H80" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L79" s="1" t="s">
+      <c r="L80" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:12">
+      <c r="A81" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G80" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="29">
-      <c r="A81" s="1" t="s">
+      <c r="G81" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="30">
+      <c r="A82" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G81" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I81" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G82" s="9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G82" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G83" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G83" s="9" t="b">
+      <c r="G84" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="H84" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L83" s="1" t="s">
+      <c r="L84" s="1" t="s">
         <v>431</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L83"/>
+  <autoFilter ref="A1:L84"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>